<commit_message>
save 19 01 2026
</commit_message>
<xml_diff>
--- a/4 четверть_18_JavaScript_pm2.xlsx
+++ b/4 четверть_18_JavaScript_pm2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlexServHW\Desktop\GB_Developer_Workbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F30D450B-BBE7-47A9-80BE-B9DABC247C9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA456BA-10CE-4A03-8E96-BFCD3BFB7070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14355" yWindow="-14820" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-13875" yWindow="-21720" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pm2" sheetId="15" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Installation</t>
   </si>
@@ -48,47 +48,6 @@
     <t>Запуск приложения</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">pm2 start </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.start/pm2_prod.json</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-pm2 start </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>prod</t>
-    </r>
-  </si>
-  <si>
     <t>Запуск приложения через указания файла main</t>
   </si>
   <si>
@@ -863,17 +822,102 @@
 &lt;----pm2 упал----&gt;</t>
     </r>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">pm2 start </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">.start/pm2_prod.json
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>pm2 save</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+pm2 start </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>prod</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Важно!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> pm2 save требуется, чтобы сохранить конфигурации из файла pm2_prod.json, примененные командой pm2 start .start/pm2_prod.json. Если не использовать команду pm2 save, то при следующей перезагрузке сервера (restart) будет применена старая версия pm2_prod.json</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1064,9 +1108,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1077,23 +1121,23 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -1102,26 +1146,29 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1413,8 +1460,8 @@
   </sheetPr>
   <dimension ref="A2:U118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1501,7 +1548,7 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="15"/>
       <c r="C7" s="18"/>
@@ -1511,13 +1558,13 @@
       <c r="A8" s="15"/>
       <c r="B8" s="15"/>
       <c r="C8" s="18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D8" s="15"/>
     </row>
     <row r="9" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="15"/>
       <c r="C9" s="18"/>
@@ -1527,13 +1574,13 @@
       <c r="A10" s="15"/>
       <c r="B10" s="15"/>
       <c r="C10" s="18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D10" s="15"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" s="19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11" s="15"/>
       <c r="C11" s="18"/>
@@ -1541,35 +1588,35 @@
     </row>
     <row r="12" spans="1:21" ht="374.4" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="18" t="s">
+      <c r="D12" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="18" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" s="15"/>
       <c r="C13" s="18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D13" s="18"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="15"/>
       <c r="C14" s="18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D14" s="18"/>
     </row>
@@ -1583,29 +1630,31 @@
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" s="18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B16" s="15"/>
       <c r="C16" s="18" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D16" s="15"/>
     </row>
     <row r="17" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="21" t="s">
-        <v>3</v>
+      <c r="A17" s="22" t="s">
+        <v>21</v>
       </c>
       <c r="B17" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="21" t="s">
-        <v>21</v>
+      <c r="D17" s="22" t="s">
+        <v>22</v>
       </c>
-      <c r="D17" s="15"/>
     </row>
     <row r="18" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B18" s="15"/>
       <c r="C18" s="15"/>

</xml_diff>